<commit_message>
LogParser update for logged data analysis
Added new methods for data analysis:
- calculate score based on user actions and machine states
- recursive processing of functions (count errors, actions, stations)
</commit_message>
<xml_diff>
--- a/OLiVE_StateMachineGR.xlsx
+++ b/OLiVE_StateMachineGR.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="420" windowWidth="16275" windowHeight="8205" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="420" windowWidth="16275" windowHeight="8205" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="2" r:id="rId1"/>
@@ -3318,9 +3318,6 @@
     <t>το ποτιστήρι</t>
   </si>
   <si>
-    <t>Πρέπει να συνδέσεις τον σωλήνα που λείπει πριν ανοίξεις τη βαλβίδα παροχής νερού</t>
-  </si>
-  <si>
     <t>Χρειάζεσαι κάποιον να προσαρμόσει το σωλήνα στη μεριά του τοίχου ενώ γυρνάς τη γωνία</t>
   </si>
   <si>
@@ -3378,9 +3375,6 @@
     <t>Δεν χρειάζεται να μεταφέρεις τα σακιά με τις ελιές προς το παρόν</t>
   </si>
   <si>
-    <t>a/waterPipe/Ένας σωλήνας που συνδέει τη δεξαμενή νερού με το λέβητα λείπει</t>
-  </si>
-  <si>
     <t>welcome</t>
   </si>
   <si>
@@ -3532,6 +3526,12 @@
   </si>
   <si>
     <t>Το δοχείο είναι γεμάτο λάδι και είναι πολύ βαρύ (80 κιλά ) για να το μεταφέρεις μόνος σου</t>
+  </si>
+  <si>
+    <t>Πρέπει να συνδέσεις το σωλήνα που λείπει πριν ανοίξεις τη βαλβίδα παροχής νερού</t>
+  </si>
+  <si>
+    <t>a/waterPipe/Λείπει ο σωλήνας που συνδέει τη δεξαμενή νερού με το λέβητα</t>
   </si>
 </sst>
 </file>
@@ -5256,7 +5256,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H316"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A276" workbookViewId="0">
+    <sheetView topLeftCell="A276" workbookViewId="0">
       <selection activeCell="F283" sqref="F283"/>
     </sheetView>
   </sheetViews>
@@ -5847,7 +5847,7 @@
         <v>793</v>
       </c>
       <c r="F30" s="80" t="s">
-        <v>1097</v>
+        <v>1095</v>
       </c>
       <c r="G30" s="80" t="s">
         <v>95</v>
@@ -5921,7 +5921,7 @@
         <v>435</v>
       </c>
       <c r="F34" s="21" t="s">
-        <v>1083</v>
+        <v>1081</v>
       </c>
       <c r="G34" s="21" t="s">
         <v>457</v>
@@ -6783,7 +6783,7 @@
         <v>183</v>
       </c>
       <c r="F80" s="21" t="s">
-        <v>1082</v>
+        <v>1080</v>
       </c>
       <c r="G80" s="21" t="s">
         <v>211</v>
@@ -9135,7 +9135,7 @@
         <v>828</v>
       </c>
       <c r="F203" s="23" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
       <c r="G203" s="23" t="s">
         <v>937</v>
@@ -9310,7 +9310,7 @@
         <v>835</v>
       </c>
       <c r="F212" s="23" t="s">
-        <v>1089</v>
+        <v>1087</v>
       </c>
       <c r="G212" s="23" t="s">
         <v>649</v>
@@ -9639,7 +9639,7 @@
         <v>827</v>
       </c>
       <c r="F229" s="23" t="s">
-        <v>1090</v>
+        <v>1088</v>
       </c>
       <c r="G229" s="23" t="s">
         <v>648</v>
@@ -9812,7 +9812,7 @@
         <v>836</v>
       </c>
       <c r="F238" s="23" t="s">
-        <v>1089</v>
+        <v>1087</v>
       </c>
       <c r="G238" s="23" t="s">
         <v>649</v>
@@ -9932,7 +9932,7 @@
         <v>295</v>
       </c>
       <c r="F245" s="2" t="s">
-        <v>1094</v>
+        <v>1092</v>
       </c>
       <c r="G245" s="2" t="s">
         <v>297</v>
@@ -10027,7 +10027,7 @@
         <v>533</v>
       </c>
       <c r="F250" s="21" t="s">
-        <v>1096</v>
+        <v>1094</v>
       </c>
       <c r="G250" s="21" t="s">
         <v>322</v>
@@ -10096,7 +10096,7 @@
         <v>305</v>
       </c>
       <c r="F254" s="21" t="s">
-        <v>1095</v>
+        <v>1093</v>
       </c>
       <c r="G254" s="21" t="s">
         <v>313</v>
@@ -10119,7 +10119,7 @@
         <v>352</v>
       </c>
       <c r="F255" s="46" t="s">
-        <v>1086</v>
+        <v>1084</v>
       </c>
       <c r="G255" s="46" t="s">
         <v>342</v>
@@ -10524,7 +10524,7 @@
         <v>564</v>
       </c>
       <c r="F277" s="38" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
       <c r="G277" s="38" t="s">
         <v>551</v>
@@ -10616,7 +10616,7 @@
         <v>729</v>
       </c>
       <c r="F282" s="2" t="s">
-        <v>1100</v>
+        <v>1098</v>
       </c>
       <c r="G282" s="2" t="s">
         <v>717</v>
@@ -10928,7 +10928,7 @@
         <v>558</v>
       </c>
       <c r="F299" s="38" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
       <c r="G299" s="38" t="s">
         <v>550</v>
@@ -11020,7 +11020,7 @@
         <v>730</v>
       </c>
       <c r="F304" s="2" t="s">
-        <v>1100</v>
+        <v>1098</v>
       </c>
       <c r="G304" s="2" t="s">
         <v>717</v>
@@ -11152,7 +11152,7 @@
         <v>374</v>
       </c>
       <c r="E311" s="4" t="s">
-        <v>1098</v>
+        <v>1096</v>
       </c>
       <c r="H311" s="70" t="s">
         <v>377</v>
@@ -11171,7 +11171,7 @@
       <c r="D312" s="19"/>
       <c r="E312" s="22"/>
       <c r="F312" s="21" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
       <c r="G312" s="21" t="s">
         <v>826</v>
@@ -11212,7 +11212,7 @@
         <v>375</v>
       </c>
       <c r="E314" s="4" t="s">
-        <v>1099</v>
+        <v>1097</v>
       </c>
       <c r="H314" s="70" t="s">
         <v>377</v>
@@ -11250,7 +11250,7 @@
         <v>378</v>
       </c>
       <c r="E316" s="4" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
     </row>
   </sheetData>
@@ -11585,101 +11585,101 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B1" t="s">
         <v>1050</v>
       </c>
-      <c r="B1" t="s">
-        <v>1052</v>
-      </c>
       <c r="C1" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>1051</v>
+      </c>
+      <c r="B2" t="s">
         <v>1053</v>
       </c>
-      <c r="B2" t="s">
-        <v>1055</v>
-      </c>
       <c r="C2" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
       <c r="B3" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
       <c r="C3" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>1056</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1057</v>
+      </c>
+      <c r="C4" t="s">
         <v>1058</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1059</v>
-      </c>
-      <c r="C4" t="s">
-        <v>1060</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1068</v>
+        <v>1066</v>
       </c>
       <c r="B5" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
       <c r="C5" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
       <c r="B6" t="s">
-        <v>1079</v>
+        <v>1077</v>
       </c>
       <c r="C6" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>1074</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C7" t="s">
         <v>1076</v>
-      </c>
-      <c r="B7" t="s">
-        <v>1080</v>
-      </c>
-      <c r="C7" t="s">
-        <v>1078</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>1068</v>
+      </c>
+      <c r="B8" t="s">
         <v>1070</v>
       </c>
-      <c r="B8" t="s">
-        <v>1072</v>
-      </c>
       <c r="C8" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>1071</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1072</v>
+      </c>
+      <c r="C9" t="s">
         <v>1073</v>
-      </c>
-      <c r="B9" t="s">
-        <v>1074</v>
-      </c>
-      <c r="C9" t="s">
-        <v>1075</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -11841,7 +11841,7 @@
         <v>469</v>
       </c>
       <c r="B24" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
       <c r="C24" t="s">
         <v>642</v>
@@ -11852,7 +11852,7 @@
         <v>472</v>
       </c>
       <c r="B25" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
       <c r="C25" t="s">
         <v>642</v>
@@ -11863,7 +11863,7 @@
         <v>491</v>
       </c>
       <c r="B26" t="s">
-        <v>1091</v>
+        <v>1089</v>
       </c>
       <c r="C26" t="s">
         <v>643</v>
@@ -11874,7 +11874,7 @@
         <v>492</v>
       </c>
       <c r="B27" t="s">
-        <v>1091</v>
+        <v>1089</v>
       </c>
       <c r="C27" t="s">
         <v>643</v>
@@ -11885,7 +11885,7 @@
         <v>536</v>
       </c>
       <c r="B28" t="s">
-        <v>1093</v>
+        <v>1091</v>
       </c>
       <c r="C28" t="s">
         <v>644</v>
@@ -11907,7 +11907,7 @@
         <v>471</v>
       </c>
       <c r="B30" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
       <c r="C30" t="s">
         <v>646</v>
@@ -11918,7 +11918,7 @@
         <v>479</v>
       </c>
       <c r="B31" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
       <c r="C31" t="s">
         <v>646</v>
@@ -11929,7 +11929,7 @@
         <v>474</v>
       </c>
       <c r="B32" t="s">
-        <v>1081</v>
+        <v>1079</v>
       </c>
       <c r="C32" t="s">
         <v>628</v>
@@ -12263,8 +12263,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12316,7 +12316,7 @@
         <v>677</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>1049</v>
+        <v>1100</v>
       </c>
       <c r="G2" s="21" t="s">
         <v>719</v>
@@ -12333,7 +12333,7 @@
         <v>89</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>1029</v>
+        <v>1099</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>663</v>
@@ -12350,7 +12350,7 @@
         <v>667</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>784</v>
@@ -12367,7 +12367,7 @@
         <v>748</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>785</v>
@@ -12384,7 +12384,7 @@
         <v>673</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>786</v>
@@ -12401,7 +12401,7 @@
         <v>668</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>787</v>
@@ -12421,7 +12421,7 @@
         <v>747</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>789</v>
@@ -12438,7 +12438,7 @@
         <v>749</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>1085</v>
+        <v>1083</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>788</v>
@@ -12461,7 +12461,7 @@
         <v>678</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>665</v>
@@ -12480,7 +12480,7 @@
       <c r="D11" s="19"/>
       <c r="E11" s="22"/>
       <c r="F11" s="21" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="G11" s="21" t="s">
         <v>666</v>
@@ -12503,7 +12503,7 @@
         <v>679</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>670</v>
@@ -12524,7 +12524,7 @@
         <v>834</v>
       </c>
       <c r="F13" s="21" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="G13" s="21" t="s">
         <v>672</v>
@@ -12541,7 +12541,7 @@
         <v>89</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>720</v>
@@ -12564,7 +12564,7 @@
         <v>689</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>685</v>
@@ -12597,7 +12597,7 @@
         <v>695</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>686</v>
@@ -12620,7 +12620,7 @@
         <v>693</v>
       </c>
       <c r="F18" s="23" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="G18" s="23" t="s">
         <v>690</v>
@@ -12652,7 +12652,7 @@
       </c>
       <c r="E20" s="22"/>
       <c r="F20" s="21" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="G20" s="21" t="s">
         <v>721</v>
@@ -12689,7 +12689,7 @@
         <v>694</v>
       </c>
       <c r="F22" s="21" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="G22" s="21" t="s">
         <v>722</v>
@@ -12727,7 +12727,7 @@
         <v>817</v>
       </c>
       <c r="F24" s="21" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="G24" s="21" t="s">
         <v>812</v>
@@ -12747,7 +12747,7 @@
         <v>818</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>807</v>
@@ -12770,7 +12770,7 @@
         <v>819</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>811</v>
@@ -12791,7 +12791,7 @@
         <v>821</v>
       </c>
       <c r="F27" s="21" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="G27" s="21" t="s">
         <v>810</v>
@@ -12810,7 +12810,7 @@
       <c r="D28" s="24"/>
       <c r="E28" s="34"/>
       <c r="F28" s="23" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="G28" s="23" t="s">
         <v>820</v>

</xml_diff>